<commit_message>
Updated FG.xlsx in Cloud
</commit_message>
<xml_diff>
--- a/Data/Inputs/FG.xlsx
+++ b/Data/Inputs/FG.xlsx
@@ -1,21 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vish_\OneDrive\Documents\UiPath\RoboticEnterpriseFramework_Excel\Data\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A67F05-B273-4D4D-89B4-5C1B23774789}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A67F05-B273-4D4D-89B4-5C1B23774789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -3569,7 +3585,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4409,9 +4425,9 @@
       <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4464,7 +4480,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -4517,7 +4533,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -4570,7 +4586,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -4623,7 +4639,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -4676,7 +4692,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -4729,7 +4745,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -4782,7 +4798,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -4835,7 +4851,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -4888,7 +4904,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -4941,7 +4957,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -4994,7 +5010,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -5047,7 +5063,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -5100,7 +5116,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -5153,7 +5169,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -5206,7 +5222,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -5259,7 +5275,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -5312,7 +5328,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -5365,7 +5381,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -5418,7 +5434,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -5471,7 +5487,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -5524,7 +5540,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -5577,7 +5593,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -5630,7 +5646,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -5683,7 +5699,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -5736,7 +5752,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -5789,7 +5805,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -5842,7 +5858,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -5895,7 +5911,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -5948,7 +5964,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -6001,7 +6017,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -6054,7 +6070,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -6107,7 +6123,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -6160,7 +6176,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -6213,7 +6229,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -6266,7 +6282,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -6319,7 +6335,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -6372,7 +6388,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -6425,7 +6441,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -6478,7 +6494,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17">
       <c r="A40" t="s">
         <v>17</v>
       </c>
@@ -6531,7 +6547,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17">
       <c r="A41" t="s">
         <v>17</v>
       </c>
@@ -6584,7 +6600,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17">
       <c r="A42" t="s">
         <v>34</v>
       </c>
@@ -6637,7 +6653,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17">
       <c r="A43" t="s">
         <v>17</v>
       </c>
@@ -6690,7 +6706,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -6743,7 +6759,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17">
       <c r="A45" t="s">
         <v>34</v>
       </c>
@@ -6796,7 +6812,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17">
       <c r="A46" t="s">
         <v>17</v>
       </c>
@@ -6849,7 +6865,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17">
       <c r="A47" t="s">
         <v>34</v>
       </c>
@@ -6902,7 +6918,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17">
       <c r="A48" t="s">
         <v>34</v>
       </c>
@@ -6955,7 +6971,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17">
       <c r="A49" t="s">
         <v>17</v>
       </c>
@@ -7008,7 +7024,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -7061,7 +7077,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17">
       <c r="A51" t="s">
         <v>34</v>
       </c>
@@ -7114,7 +7130,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17">
       <c r="A52" t="s">
         <v>17</v>
       </c>
@@ -7167,7 +7183,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17">
       <c r="A53" t="s">
         <v>34</v>
       </c>
@@ -7220,7 +7236,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17">
       <c r="A54" t="s">
         <v>17</v>
       </c>
@@ -7273,7 +7289,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17">
       <c r="A55" t="s">
         <v>34</v>
       </c>
@@ -7326,7 +7342,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17">
       <c r="A56" t="s">
         <v>17</v>
       </c>
@@ -7379,7 +7395,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17">
       <c r="A57" t="s">
         <v>34</v>
       </c>
@@ -7432,7 +7448,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17">
       <c r="A58" t="s">
         <v>17</v>
       </c>
@@ -7485,7 +7501,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17">
       <c r="A59" t="s">
         <v>34</v>
       </c>
@@ -7538,7 +7554,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17">
       <c r="A60" t="s">
         <v>17</v>
       </c>
@@ -7591,7 +7607,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17">
       <c r="A61" t="s">
         <v>34</v>
       </c>
@@ -7644,7 +7660,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17">
       <c r="A62" t="s">
         <v>17</v>
       </c>
@@ -7697,7 +7713,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17">
       <c r="A63" t="s">
         <v>17</v>
       </c>
@@ -7750,7 +7766,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17">
       <c r="A64" t="s">
         <v>34</v>
       </c>
@@ -7803,7 +7819,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17">
       <c r="A65" t="s">
         <v>34</v>
       </c>
@@ -7856,7 +7872,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17">
       <c r="A66" t="s">
         <v>17</v>
       </c>
@@ -7909,7 +7925,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17">
       <c r="A67" t="s">
         <v>34</v>
       </c>
@@ -7962,7 +7978,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17">
       <c r="A68" t="s">
         <v>34</v>
       </c>
@@ -8015,7 +8031,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17">
       <c r="A69" t="s">
         <v>34</v>
       </c>
@@ -8068,7 +8084,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17">
       <c r="A70" t="s">
         <v>17</v>
       </c>
@@ -8121,7 +8137,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17">
       <c r="A71" t="s">
         <v>34</v>
       </c>
@@ -8174,7 +8190,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17">
       <c r="A72" t="s">
         <v>17</v>
       </c>
@@ -8227,7 +8243,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17">
       <c r="A73" t="s">
         <v>17</v>
       </c>
@@ -8280,7 +8296,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17">
       <c r="A74" t="s">
         <v>17</v>
       </c>
@@ -8333,7 +8349,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17">
       <c r="A75" t="s">
         <v>34</v>
       </c>
@@ -8386,7 +8402,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17">
       <c r="A76" t="s">
         <v>17</v>
       </c>
@@ -8439,7 +8455,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17">
       <c r="A77" t="s">
         <v>34</v>
       </c>
@@ -8492,7 +8508,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17">
       <c r="A78" t="s">
         <v>17</v>
       </c>
@@ -8545,7 +8561,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17">
       <c r="A79" t="s">
         <v>17</v>
       </c>
@@ -8598,7 +8614,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17">
       <c r="A80" t="s">
         <v>17</v>
       </c>
@@ -8651,7 +8667,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17">
       <c r="A81" t="s">
         <v>34</v>
       </c>
@@ -8704,7 +8720,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17">
       <c r="A82" t="s">
         <v>17</v>
       </c>
@@ -8757,7 +8773,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17">
       <c r="A83" t="s">
         <v>34</v>
       </c>
@@ -8810,7 +8826,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17">
       <c r="A84" t="s">
         <v>17</v>
       </c>
@@ -8863,7 +8879,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17">
       <c r="A85" t="s">
         <v>17</v>
       </c>
@@ -8916,7 +8932,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17">
       <c r="A86" t="s">
         <v>17</v>
       </c>
@@ -8969,7 +8985,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17">
       <c r="A87" t="s">
         <v>17</v>
       </c>
@@ -9022,7 +9038,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17">
       <c r="A88" t="s">
         <v>34</v>
       </c>
@@ -9075,7 +9091,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17">
       <c r="A89" t="s">
         <v>17</v>
       </c>
@@ -9128,7 +9144,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17">
       <c r="A90" t="s">
         <v>34</v>
       </c>
@@ -9181,7 +9197,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17">
       <c r="A91" t="s">
         <v>17</v>
       </c>
@@ -9234,7 +9250,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17">
       <c r="A92" t="s">
         <v>17</v>
       </c>
@@ -9287,7 +9303,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17">
       <c r="A93" t="s">
         <v>17</v>
       </c>
@@ -9340,7 +9356,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17">
       <c r="A94" t="s">
         <v>17</v>
       </c>
@@ -9393,7 +9409,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17">
       <c r="A95" t="s">
         <v>17</v>
       </c>
@@ -9446,7 +9462,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17">
       <c r="A96" t="s">
         <v>17</v>
       </c>
@@ -9499,7 +9515,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17">
       <c r="A97" t="s">
         <v>34</v>
       </c>
@@ -9552,7 +9568,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:17">
       <c r="A98" t="s">
         <v>17</v>
       </c>
@@ -9605,7 +9621,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17">
       <c r="A99" t="s">
         <v>34</v>
       </c>
@@ -9658,7 +9674,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17">
       <c r="A100" t="s">
         <v>17</v>
       </c>
@@ -9711,7 +9727,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17">
       <c r="A101" t="s">
         <v>34</v>
       </c>

</xml_diff>